<commit_message>
Big edit, added statistics, repaired some errors
</commit_message>
<xml_diff>
--- a/Wyniki/Tabele/jakosc_gleby.xlsx
+++ b/Wyniki/Tabele/jakosc_gleby.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="6">
   <si>
     <t>Pole</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Nebbiolo</t>
+  </si>
+  <si>
+    <t>Arneis</t>
+  </si>
+  <si>
+    <t>Dolcetto</t>
   </si>
 </sst>
 </file>
@@ -394,13 +400,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,47 +419,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2483063555949173</v>
+        <v>0.2292229449333333</v>
       </c>
       <c r="C2">
-        <v>0.2759155643566499</v>
+        <v>0.2120378030483504</v>
       </c>
       <c r="D2">
-        <v>0.2273482024847029</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.2694120714877833</v>
+      </c>
+      <c r="E2">
+        <v>0.2662591042135437</v>
+      </c>
+      <c r="F2">
+        <v>0.2833381417234191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2731252547274299</v>
+        <v>0.2262785370937492</v>
       </c>
       <c r="C3">
-        <v>0.2630348218903652</v>
+        <v>0.2431984596261966</v>
       </c>
       <c r="D3">
-        <v>0.2510506278291808</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.2231242816054936</v>
+      </c>
+      <c r="E3">
+        <v>0.2600746786059626</v>
+      </c>
+      <c r="F3">
+        <v>0.2694364887074815</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2148893732835294</v>
+        <v>0.2843159874191754</v>
       </c>
       <c r="C4">
-        <v>0.2382436807735286</v>
+        <v>0.2762147332896926</v>
       </c>
       <c r="D4">
-        <v>0.2585341084374443</v>
+        <v>0.2362805672010626</v>
+      </c>
+      <c r="E4">
+        <v>0.2838887570009956</v>
+      </c>
+      <c r="F4">
+        <v>0.2541915502597359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.2793730657447849</v>
+      </c>
+      <c r="C5">
+        <v>0.2754236429072471</v>
+      </c>
+      <c r="D5">
+        <v>0.2244896851041773</v>
+      </c>
+      <c r="E5">
+        <v>0.2401628214429717</v>
+      </c>
+      <c r="F5">
+        <v>0.211714624672996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.2406454138497441</v>
+      </c>
+      <c r="C6">
+        <v>0.251487014980054</v>
+      </c>
+      <c r="D6">
+        <v>0.236236043124155</v>
+      </c>
+      <c r="E6">
+        <v>0.2431195653486732</v>
+      </c>
+      <c r="F6">
+        <v>0.2248638010183419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.2711386462558246</v>
+      </c>
+      <c r="C7">
+        <v>0.2485307380119831</v>
+      </c>
+      <c r="D7">
+        <v>0.2603219824825472</v>
+      </c>
+      <c r="E7">
+        <v>0.2123866913617174</v>
+      </c>
+      <c r="F7">
+        <v>0.2189284007752328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.2789839242165219</v>
+      </c>
+      <c r="C8">
+        <v>0.2768909761304083</v>
+      </c>
+      <c r="D8">
+        <v>0.2356882859520498</v>
+      </c>
+      <c r="E8">
+        <v>0.2581709760600411</v>
+      </c>
+      <c r="F8">
+        <v>0.2555960761131025</v>
       </c>
     </row>
   </sheetData>
@@ -463,13 +573,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,47 +592,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5793814963881404</v>
+        <v>0.5348535381777776</v>
       </c>
       <c r="C2">
-        <v>0.6438029834988499</v>
+        <v>0.4947548737794842</v>
       </c>
       <c r="D2">
-        <v>0.5304791391309733</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6286281668048278</v>
+      </c>
+      <c r="E2">
+        <v>0.6212712431649353</v>
+      </c>
+      <c r="F2">
+        <v>0.6611223306879779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6372922610306697</v>
+        <v>0.5279832532187482</v>
       </c>
       <c r="C3">
-        <v>0.6137479177441855</v>
+        <v>0.5674630724611255</v>
       </c>
       <c r="D3">
-        <v>0.5857847982680885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.5206233237461516</v>
+      </c>
+      <c r="E3">
+        <v>0.6068409167472462</v>
+      </c>
+      <c r="F3">
+        <v>0.6286851403174569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5014085376615687</v>
+        <v>0.6634039706447424</v>
       </c>
       <c r="C4">
-        <v>0.5559019218049001</v>
+        <v>0.644501044342616</v>
       </c>
       <c r="D4">
-        <v>0.6032462530207034</v>
+        <v>0.551321323469146</v>
+      </c>
+      <c r="E4">
+        <v>0.6624070996689898</v>
+      </c>
+      <c r="F4">
+        <v>0.5931136172727171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6518704867378313</v>
+      </c>
+      <c r="C5">
+        <v>0.6426551667835766</v>
+      </c>
+      <c r="D5">
+        <v>0.5238092652430802</v>
+      </c>
+      <c r="E5">
+        <v>0.5603799167002674</v>
+      </c>
+      <c r="F5">
+        <v>0.4940007909036573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5615059656494029</v>
+      </c>
+      <c r="C6">
+        <v>0.5868030349534594</v>
+      </c>
+      <c r="D6">
+        <v>0.5512174339563617</v>
+      </c>
+      <c r="E6">
+        <v>0.5672789858135707</v>
+      </c>
+      <c r="F6">
+        <v>0.5246822023761311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.6326568412635906</v>
+      </c>
+      <c r="C7">
+        <v>0.5799050553612939</v>
+      </c>
+      <c r="D7">
+        <v>0.6074179591259434</v>
+      </c>
+      <c r="E7">
+        <v>0.4955689465106738</v>
+      </c>
+      <c r="F7">
+        <v>0.5108329351422098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.650962489838551</v>
+      </c>
+      <c r="C8">
+        <v>0.6460789443042859</v>
+      </c>
+      <c r="D8">
+        <v>0.5499393338881162</v>
+      </c>
+      <c r="E8">
+        <v>0.6023989441400958</v>
+      </c>
+      <c r="F8">
+        <v>0.5963908442639059</v>
       </c>
     </row>
   </sheetData>
@@ -532,13 +746,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,47 +765,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.8276878519830577</v>
+        <v>0.7640764831111109</v>
       </c>
       <c r="C2">
-        <v>0.9197185478554999</v>
+        <v>0.7067926768278346</v>
       </c>
       <c r="D2">
-        <v>0.7578273416156762</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.8980402382926111</v>
+      </c>
+      <c r="E2">
+        <v>0.8875303473784791</v>
+      </c>
+      <c r="F2">
+        <v>0.944460472411397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.9104175157580996</v>
+        <v>0.7542617903124974</v>
       </c>
       <c r="C3">
-        <v>0.8767827396345508</v>
+        <v>0.8106615320873222</v>
       </c>
       <c r="D3">
-        <v>0.8368354260972694</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.7437476053516452</v>
+      </c>
+      <c r="E3">
+        <v>0.8669155953532088</v>
+      </c>
+      <c r="F3">
+        <v>0.8981216290249385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7162979109450982</v>
+        <v>0.9477199580639178</v>
       </c>
       <c r="C4">
-        <v>0.7941456025784287</v>
+        <v>0.9207157776323087</v>
       </c>
       <c r="D4">
-        <v>0.8617803614581478</v>
+        <v>0.7876018906702086</v>
+      </c>
+      <c r="E4">
+        <v>0.9462958566699855</v>
+      </c>
+      <c r="F4">
+        <v>0.847305167532453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.9312435524826163</v>
+      </c>
+      <c r="C5">
+        <v>0.9180788096908238</v>
+      </c>
+      <c r="D5">
+        <v>0.7482989503472576</v>
+      </c>
+      <c r="E5">
+        <v>0.8005427381432392</v>
+      </c>
+      <c r="F5">
+        <v>0.7057154155766534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.8021513794991471</v>
+      </c>
+      <c r="C6">
+        <v>0.8382900499335135</v>
+      </c>
+      <c r="D6">
+        <v>0.7874534770805168</v>
+      </c>
+      <c r="E6">
+        <v>0.810398551162244</v>
+      </c>
+      <c r="F6">
+        <v>0.749546003394473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.9037954875194152</v>
+      </c>
+      <c r="C7">
+        <v>0.828435793373277</v>
+      </c>
+      <c r="D7">
+        <v>0.8677399416084907</v>
+      </c>
+      <c r="E7">
+        <v>0.7079556378723912</v>
+      </c>
+      <c r="F7">
+        <v>0.7297613359174426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.9299464140550728</v>
+      </c>
+      <c r="C8">
+        <v>0.9229699204346942</v>
+      </c>
+      <c r="D8">
+        <v>0.785627619840166</v>
+      </c>
+      <c r="E8">
+        <v>0.8605699202001369</v>
+      </c>
+      <c r="F8">
+        <v>0.8519869203770085</v>
       </c>
     </row>
   </sheetData>
@@ -601,13 +919,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,47 +938,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2483063555949173</v>
+        <v>0.2292229449333333</v>
       </c>
       <c r="C2">
-        <v>0.2759155643566499</v>
+        <v>0.2120378030483504</v>
       </c>
       <c r="D2">
-        <v>0.2273482024847029</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.2694120714877833</v>
+      </c>
+      <c r="E2">
+        <v>0.2662591042135437</v>
+      </c>
+      <c r="F2">
+        <v>0.2833381417234191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2731252547274299</v>
+        <v>0.2262785370937492</v>
       </c>
       <c r="C3">
-        <v>0.2630348218903652</v>
+        <v>0.2431984596261966</v>
       </c>
       <c r="D3">
-        <v>0.2510506278291808</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.2231242816054936</v>
+      </c>
+      <c r="E3">
+        <v>0.2600746786059626</v>
+      </c>
+      <c r="F3">
+        <v>0.2694364887074815</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2148893732835294</v>
+        <v>0.2843159874191754</v>
       </c>
       <c r="C4">
-        <v>0.2382436807735286</v>
+        <v>0.2762147332896926</v>
       </c>
       <c r="D4">
-        <v>0.2585341084374443</v>
+        <v>0.2362805672010626</v>
+      </c>
+      <c r="E4">
+        <v>0.2838887570009956</v>
+      </c>
+      <c r="F4">
+        <v>0.2541915502597359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.2793730657447849</v>
+      </c>
+      <c r="C5">
+        <v>0.2754236429072471</v>
+      </c>
+      <c r="D5">
+        <v>0.2244896851041773</v>
+      </c>
+      <c r="E5">
+        <v>0.2401628214429717</v>
+      </c>
+      <c r="F5">
+        <v>0.211714624672996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.2406454138497441</v>
+      </c>
+      <c r="C6">
+        <v>0.251487014980054</v>
+      </c>
+      <c r="D6">
+        <v>0.236236043124155</v>
+      </c>
+      <c r="E6">
+        <v>0.2431195653486732</v>
+      </c>
+      <c r="F6">
+        <v>0.2248638010183419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.2711386462558246</v>
+      </c>
+      <c r="C7">
+        <v>0.2485307380119831</v>
+      </c>
+      <c r="D7">
+        <v>0.2603219824825472</v>
+      </c>
+      <c r="E7">
+        <v>0.2123866913617174</v>
+      </c>
+      <c r="F7">
+        <v>0.2189284007752328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.2789839242165219</v>
+      </c>
+      <c r="C8">
+        <v>0.2768909761304083</v>
+      </c>
+      <c r="D8">
+        <v>0.2356882859520498</v>
+      </c>
+      <c r="E8">
+        <v>0.2581709760600411</v>
+      </c>
+      <c r="F8">
+        <v>0.2555960761131025</v>
       </c>
     </row>
   </sheetData>
@@ -670,13 +1092,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,47 +1111,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2483063555949173</v>
+        <v>0.2292229449333333</v>
       </c>
       <c r="C2">
-        <v>0.2759155643566499</v>
+        <v>0.2120378030483504</v>
       </c>
       <c r="D2">
-        <v>0.2273482024847029</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.2694120714877833</v>
+      </c>
+      <c r="E2">
+        <v>0.2662591042135437</v>
+      </c>
+      <c r="F2">
+        <v>0.2833381417234191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2731252547274299</v>
+        <v>0.2262785370937492</v>
       </c>
       <c r="C3">
-        <v>0.2630348218903652</v>
+        <v>0.2431984596261966</v>
       </c>
       <c r="D3">
-        <v>0.2510506278291808</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.2231242816054936</v>
+      </c>
+      <c r="E3">
+        <v>0.2600746786059626</v>
+      </c>
+      <c r="F3">
+        <v>0.2694364887074815</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2148893732835294</v>
+        <v>0.2843159874191754</v>
       </c>
       <c r="C4">
-        <v>0.2382436807735286</v>
+        <v>0.2762147332896926</v>
       </c>
       <c r="D4">
-        <v>0.2585341084374443</v>
+        <v>0.2362805672010626</v>
+      </c>
+      <c r="E4">
+        <v>0.2838887570009956</v>
+      </c>
+      <c r="F4">
+        <v>0.2541915502597359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.2793730657447849</v>
+      </c>
+      <c r="C5">
+        <v>0.2754236429072471</v>
+      </c>
+      <c r="D5">
+        <v>0.2244896851041773</v>
+      </c>
+      <c r="E5">
+        <v>0.2401628214429717</v>
+      </c>
+      <c r="F5">
+        <v>0.211714624672996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.2406454138497441</v>
+      </c>
+      <c r="C6">
+        <v>0.251487014980054</v>
+      </c>
+      <c r="D6">
+        <v>0.236236043124155</v>
+      </c>
+      <c r="E6">
+        <v>0.2431195653486732</v>
+      </c>
+      <c r="F6">
+        <v>0.2248638010183419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.2711386462558246</v>
+      </c>
+      <c r="C7">
+        <v>0.2485307380119831</v>
+      </c>
+      <c r="D7">
+        <v>0.2603219824825472</v>
+      </c>
+      <c r="E7">
+        <v>0.2123866913617174</v>
+      </c>
+      <c r="F7">
+        <v>0.2189284007752328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.2789839242165219</v>
+      </c>
+      <c r="C8">
+        <v>0.2768909761304083</v>
+      </c>
+      <c r="D8">
+        <v>0.2356882859520498</v>
+      </c>
+      <c r="E8">
+        <v>0.2581709760600411</v>
+      </c>
+      <c r="F8">
+        <v>0.2555960761131025</v>
       </c>
     </row>
   </sheetData>
@@ -739,13 +1265,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,47 +1284,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.8276878519830577</v>
+        <v>0.7640764831111109</v>
       </c>
       <c r="C2">
-        <v>0.9197185478554999</v>
+        <v>0.7067926768278346</v>
       </c>
       <c r="D2">
-        <v>0.7578273416156762</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.8980402382926111</v>
+      </c>
+      <c r="E2">
+        <v>0.8875303473784791</v>
+      </c>
+      <c r="F2">
+        <v>0.944460472411397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.9104175157580996</v>
+        <v>0.7542617903124974</v>
       </c>
       <c r="C3">
-        <v>0.8767827396345508</v>
+        <v>0.8106615320873222</v>
       </c>
       <c r="D3">
-        <v>0.8368354260972694</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.7437476053516452</v>
+      </c>
+      <c r="E3">
+        <v>0.8669155953532088</v>
+      </c>
+      <c r="F3">
+        <v>0.8981216290249385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7162979109450982</v>
+        <v>0.9477199580639178</v>
       </c>
       <c r="C4">
-        <v>0.7941456025784287</v>
+        <v>0.9207157776323087</v>
       </c>
       <c r="D4">
-        <v>0.8617803614581478</v>
+        <v>0.7876018906702086</v>
+      </c>
+      <c r="E4">
+        <v>0.9462958566699855</v>
+      </c>
+      <c r="F4">
+        <v>0.847305167532453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.9312435524826163</v>
+      </c>
+      <c r="C5">
+        <v>0.9180788096908238</v>
+      </c>
+      <c r="D5">
+        <v>0.7482989503472576</v>
+      </c>
+      <c r="E5">
+        <v>0.8005427381432392</v>
+      </c>
+      <c r="F5">
+        <v>0.7057154155766534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.8021513794991471</v>
+      </c>
+      <c r="C6">
+        <v>0.8382900499335135</v>
+      </c>
+      <c r="D6">
+        <v>0.7874534770805168</v>
+      </c>
+      <c r="E6">
+        <v>0.810398551162244</v>
+      </c>
+      <c r="F6">
+        <v>0.749546003394473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.9037954875194152</v>
+      </c>
+      <c r="C7">
+        <v>0.828435793373277</v>
+      </c>
+      <c r="D7">
+        <v>0.8677399416084907</v>
+      </c>
+      <c r="E7">
+        <v>0.7079556378723912</v>
+      </c>
+      <c r="F7">
+        <v>0.7297613359174426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.9299464140550728</v>
+      </c>
+      <c r="C8">
+        <v>0.9229699204346942</v>
+      </c>
+      <c r="D8">
+        <v>0.785627619840166</v>
+      </c>
+      <c r="E8">
+        <v>0.8605699202001369</v>
+      </c>
+      <c r="F8">
+        <v>0.8519869203770085</v>
       </c>
     </row>
   </sheetData>
@@ -808,13 +1438,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,47 +1457,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5793814963881404</v>
+        <v>0.5348535381777776</v>
       </c>
       <c r="C2">
-        <v>0.6438029834988499</v>
+        <v>0.4947548737794842</v>
       </c>
       <c r="D2">
-        <v>0.5304791391309733</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6286281668048278</v>
+      </c>
+      <c r="E2">
+        <v>0.6212712431649353</v>
+      </c>
+      <c r="F2">
+        <v>0.6611223306879779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6372922610306697</v>
+        <v>0.5279832532187482</v>
       </c>
       <c r="C3">
-        <v>0.6137479177441855</v>
+        <v>0.5674630724611255</v>
       </c>
       <c r="D3">
-        <v>0.5857847982680885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.5206233237461516</v>
+      </c>
+      <c r="E3">
+        <v>0.6068409167472462</v>
+      </c>
+      <c r="F3">
+        <v>0.6286851403174569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5014085376615687</v>
+        <v>0.6634039706447424</v>
       </c>
       <c r="C4">
-        <v>0.5559019218049001</v>
+        <v>0.644501044342616</v>
       </c>
       <c r="D4">
-        <v>0.6032462530207034</v>
+        <v>0.551321323469146</v>
+      </c>
+      <c r="E4">
+        <v>0.6624070996689898</v>
+      </c>
+      <c r="F4">
+        <v>0.5931136172727171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6518704867378313</v>
+      </c>
+      <c r="C5">
+        <v>0.6426551667835766</v>
+      </c>
+      <c r="D5">
+        <v>0.5238092652430802</v>
+      </c>
+      <c r="E5">
+        <v>0.5603799167002674</v>
+      </c>
+      <c r="F5">
+        <v>0.4940007909036573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5615059656494029</v>
+      </c>
+      <c r="C6">
+        <v>0.5868030349534594</v>
+      </c>
+      <c r="D6">
+        <v>0.5512174339563617</v>
+      </c>
+      <c r="E6">
+        <v>0.5672789858135707</v>
+      </c>
+      <c r="F6">
+        <v>0.5246822023761311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.6326568412635906</v>
+      </c>
+      <c r="C7">
+        <v>0.5799050553612939</v>
+      </c>
+      <c r="D7">
+        <v>0.6074179591259434</v>
+      </c>
+      <c r="E7">
+        <v>0.4955689465106738</v>
+      </c>
+      <c r="F7">
+        <v>0.5108329351422098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.650962489838551</v>
+      </c>
+      <c r="C8">
+        <v>0.6460789443042859</v>
+      </c>
+      <c r="D8">
+        <v>0.5499393338881162</v>
+      </c>
+      <c r="E8">
+        <v>0.6023989441400958</v>
+      </c>
+      <c r="F8">
+        <v>0.5963908442639059</v>
       </c>
     </row>
   </sheetData>
@@ -877,13 +1611,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,47 +1630,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5793814963881404</v>
+        <v>0.5348535381777776</v>
       </c>
       <c r="C2">
-        <v>0.6438029834988499</v>
+        <v>0.4947548737794842</v>
       </c>
       <c r="D2">
-        <v>0.5304791391309733</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6286281668048278</v>
+      </c>
+      <c r="E2">
+        <v>0.6212712431649353</v>
+      </c>
+      <c r="F2">
+        <v>0.6611223306879779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6372922610306697</v>
+        <v>0.5279832532187482</v>
       </c>
       <c r="C3">
-        <v>0.6137479177441855</v>
+        <v>0.5674630724611255</v>
       </c>
       <c r="D3">
-        <v>0.5857847982680885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.5206233237461516</v>
+      </c>
+      <c r="E3">
+        <v>0.6068409167472462</v>
+      </c>
+      <c r="F3">
+        <v>0.6286851403174569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5014085376615687</v>
+        <v>0.6634039706447424</v>
       </c>
       <c r="C4">
-        <v>0.5559019218049001</v>
+        <v>0.644501044342616</v>
       </c>
       <c r="D4">
-        <v>0.6032462530207034</v>
+        <v>0.551321323469146</v>
+      </c>
+      <c r="E4">
+        <v>0.6624070996689898</v>
+      </c>
+      <c r="F4">
+        <v>0.5931136172727171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6518704867378313</v>
+      </c>
+      <c r="C5">
+        <v>0.6426551667835766</v>
+      </c>
+      <c r="D5">
+        <v>0.5238092652430802</v>
+      </c>
+      <c r="E5">
+        <v>0.5603799167002674</v>
+      </c>
+      <c r="F5">
+        <v>0.4940007909036573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5615059656494029</v>
+      </c>
+      <c r="C6">
+        <v>0.5868030349534594</v>
+      </c>
+      <c r="D6">
+        <v>0.5512174339563617</v>
+      </c>
+      <c r="E6">
+        <v>0.5672789858135707</v>
+      </c>
+      <c r="F6">
+        <v>0.5246822023761311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.6326568412635906</v>
+      </c>
+      <c r="C7">
+        <v>0.5799050553612939</v>
+      </c>
+      <c r="D7">
+        <v>0.6074179591259434</v>
+      </c>
+      <c r="E7">
+        <v>0.4955689465106738</v>
+      </c>
+      <c r="F7">
+        <v>0.5108329351422098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.650962489838551</v>
+      </c>
+      <c r="C8">
+        <v>0.6460789443042859</v>
+      </c>
+      <c r="D8">
+        <v>0.5499393338881162</v>
+      </c>
+      <c r="E8">
+        <v>0.6023989441400958</v>
+      </c>
+      <c r="F8">
+        <v>0.5963908442639059</v>
       </c>
     </row>
   </sheetData>
@@ -946,13 +1784,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,47 +1803,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5793814963881404</v>
+        <v>0.5348535381777776</v>
       </c>
       <c r="C2">
-        <v>0.6438029834988499</v>
+        <v>0.4947548737794842</v>
       </c>
       <c r="D2">
-        <v>0.5304791391309733</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6286281668048278</v>
+      </c>
+      <c r="E2">
+        <v>0.6212712431649353</v>
+      </c>
+      <c r="F2">
+        <v>0.6611223306879779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6372922610306697</v>
+        <v>0.5279832532187482</v>
       </c>
       <c r="C3">
-        <v>0.6137479177441855</v>
+        <v>0.5674630724611255</v>
       </c>
       <c r="D3">
-        <v>0.5857847982680885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.5206233237461516</v>
+      </c>
+      <c r="E3">
+        <v>0.6068409167472462</v>
+      </c>
+      <c r="F3">
+        <v>0.6286851403174569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5014085376615687</v>
+        <v>0.6634039706447424</v>
       </c>
       <c r="C4">
-        <v>0.5559019218049001</v>
+        <v>0.644501044342616</v>
       </c>
       <c r="D4">
-        <v>0.6032462530207034</v>
+        <v>0.551321323469146</v>
+      </c>
+      <c r="E4">
+        <v>0.6624070996689898</v>
+      </c>
+      <c r="F4">
+        <v>0.5931136172727171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6518704867378313</v>
+      </c>
+      <c r="C5">
+        <v>0.6426551667835766</v>
+      </c>
+      <c r="D5">
+        <v>0.5238092652430802</v>
+      </c>
+      <c r="E5">
+        <v>0.5603799167002674</v>
+      </c>
+      <c r="F5">
+        <v>0.4940007909036573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5615059656494029</v>
+      </c>
+      <c r="C6">
+        <v>0.5868030349534594</v>
+      </c>
+      <c r="D6">
+        <v>0.5512174339563617</v>
+      </c>
+      <c r="E6">
+        <v>0.5672789858135707</v>
+      </c>
+      <c r="F6">
+        <v>0.5246822023761311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.6326568412635906</v>
+      </c>
+      <c r="C7">
+        <v>0.5799050553612939</v>
+      </c>
+      <c r="D7">
+        <v>0.6074179591259434</v>
+      </c>
+      <c r="E7">
+        <v>0.4955689465106738</v>
+      </c>
+      <c r="F7">
+        <v>0.5108329351422098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.650962489838551</v>
+      </c>
+      <c r="C8">
+        <v>0.6460789443042859</v>
+      </c>
+      <c r="D8">
+        <v>0.5499393338881162</v>
+      </c>
+      <c r="E8">
+        <v>0.6023989441400958</v>
+      </c>
+      <c r="F8">
+        <v>0.5963908442639059</v>
       </c>
     </row>
   </sheetData>
@@ -1015,13 +1957,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,47 +1976,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.8276878519830577</v>
+        <v>0.7640764831111109</v>
       </c>
       <c r="C2">
-        <v>0.9197185478554999</v>
+        <v>0.7067926768278346</v>
       </c>
       <c r="D2">
-        <v>0.7578273416156762</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.8980402382926111</v>
+      </c>
+      <c r="E2">
+        <v>0.8875303473784791</v>
+      </c>
+      <c r="F2">
+        <v>0.944460472411397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.9104175157580996</v>
+        <v>0.7542617903124974</v>
       </c>
       <c r="C3">
-        <v>0.8767827396345508</v>
+        <v>0.8106615320873222</v>
       </c>
       <c r="D3">
-        <v>0.8368354260972694</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.7437476053516452</v>
+      </c>
+      <c r="E3">
+        <v>0.8669155953532088</v>
+      </c>
+      <c r="F3">
+        <v>0.8981216290249385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7162979109450982</v>
+        <v>0.9477199580639178</v>
       </c>
       <c r="C4">
-        <v>0.7941456025784287</v>
+        <v>0.9207157776323087</v>
       </c>
       <c r="D4">
-        <v>0.8617803614581478</v>
+        <v>0.7876018906702086</v>
+      </c>
+      <c r="E4">
+        <v>0.9462958566699855</v>
+      </c>
+      <c r="F4">
+        <v>0.847305167532453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.9312435524826163</v>
+      </c>
+      <c r="C5">
+        <v>0.9180788096908238</v>
+      </c>
+      <c r="D5">
+        <v>0.7482989503472576</v>
+      </c>
+      <c r="E5">
+        <v>0.8005427381432392</v>
+      </c>
+      <c r="F5">
+        <v>0.7057154155766534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.8021513794991471</v>
+      </c>
+      <c r="C6">
+        <v>0.8382900499335135</v>
+      </c>
+      <c r="D6">
+        <v>0.7874534770805168</v>
+      </c>
+      <c r="E6">
+        <v>0.810398551162244</v>
+      </c>
+      <c r="F6">
+        <v>0.749546003394473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.9037954875194152</v>
+      </c>
+      <c r="C7">
+        <v>0.828435793373277</v>
+      </c>
+      <c r="D7">
+        <v>0.8677399416084907</v>
+      </c>
+      <c r="E7">
+        <v>0.7079556378723912</v>
+      </c>
+      <c r="F7">
+        <v>0.7297613359174426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.9299464140550728</v>
+      </c>
+      <c r="C8">
+        <v>0.9229699204346942</v>
+      </c>
+      <c r="D8">
+        <v>0.785627619840166</v>
+      </c>
+      <c r="E8">
+        <v>0.8605699202001369</v>
+      </c>
+      <c r="F8">
+        <v>0.8519869203770085</v>
       </c>
     </row>
   </sheetData>
@@ -1084,13 +2130,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,47 +2149,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5793814963881404</v>
+        <v>0.5348535381777776</v>
       </c>
       <c r="C2">
-        <v>0.6438029834988499</v>
+        <v>0.4947548737794842</v>
       </c>
       <c r="D2">
-        <v>0.5304791391309733</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6286281668048278</v>
+      </c>
+      <c r="E2">
+        <v>0.6212712431649353</v>
+      </c>
+      <c r="F2">
+        <v>0.6611223306879779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6372922610306697</v>
+        <v>0.5279832532187482</v>
       </c>
       <c r="C3">
-        <v>0.6137479177441855</v>
+        <v>0.5674630724611255</v>
       </c>
       <c r="D3">
-        <v>0.5857847982680885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.5206233237461516</v>
+      </c>
+      <c r="E3">
+        <v>0.6068409167472462</v>
+      </c>
+      <c r="F3">
+        <v>0.6286851403174569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5014085376615687</v>
+        <v>0.6634039706447424</v>
       </c>
       <c r="C4">
-        <v>0.5559019218049001</v>
+        <v>0.644501044342616</v>
       </c>
       <c r="D4">
-        <v>0.6032462530207034</v>
+        <v>0.551321323469146</v>
+      </c>
+      <c r="E4">
+        <v>0.6624070996689898</v>
+      </c>
+      <c r="F4">
+        <v>0.5931136172727171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6518704867378313</v>
+      </c>
+      <c r="C5">
+        <v>0.6426551667835766</v>
+      </c>
+      <c r="D5">
+        <v>0.5238092652430802</v>
+      </c>
+      <c r="E5">
+        <v>0.5603799167002674</v>
+      </c>
+      <c r="F5">
+        <v>0.4940007909036573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5615059656494029</v>
+      </c>
+      <c r="C6">
+        <v>0.5868030349534594</v>
+      </c>
+      <c r="D6">
+        <v>0.5512174339563617</v>
+      </c>
+      <c r="E6">
+        <v>0.5672789858135707</v>
+      </c>
+      <c r="F6">
+        <v>0.5246822023761311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.6326568412635906</v>
+      </c>
+      <c r="C7">
+        <v>0.5799050553612939</v>
+      </c>
+      <c r="D7">
+        <v>0.6074179591259434</v>
+      </c>
+      <c r="E7">
+        <v>0.4955689465106738</v>
+      </c>
+      <c r="F7">
+        <v>0.5108329351422098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.650962489838551</v>
+      </c>
+      <c r="C8">
+        <v>0.6460789443042859</v>
+      </c>
+      <c r="D8">
+        <v>0.5499393338881162</v>
+      </c>
+      <c r="E8">
+        <v>0.6023989441400958</v>
+      </c>
+      <c r="F8">
+        <v>0.5963908442639059</v>
       </c>
     </row>
   </sheetData>
@@ -1153,13 +2303,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1172,47 +2322,151 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5793814963881404</v>
+        <v>0.5348535381777776</v>
       </c>
       <c r="C2">
-        <v>0.6438029834988499</v>
+        <v>0.4947548737794842</v>
       </c>
       <c r="D2">
-        <v>0.5304791391309733</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6286281668048278</v>
+      </c>
+      <c r="E2">
+        <v>0.6212712431649353</v>
+      </c>
+      <c r="F2">
+        <v>0.6611223306879779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.6372922610306697</v>
+        <v>0.5279832532187482</v>
       </c>
       <c r="C3">
-        <v>0.6137479177441855</v>
+        <v>0.5674630724611255</v>
       </c>
       <c r="D3">
-        <v>0.5857847982680885</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.5206233237461516</v>
+      </c>
+      <c r="E3">
+        <v>0.6068409167472462</v>
+      </c>
+      <c r="F3">
+        <v>0.6286851403174569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.5014085376615687</v>
+        <v>0.6634039706447424</v>
       </c>
       <c r="C4">
-        <v>0.5559019218049001</v>
+        <v>0.644501044342616</v>
       </c>
       <c r="D4">
-        <v>0.6032462530207034</v>
+        <v>0.551321323469146</v>
+      </c>
+      <c r="E4">
+        <v>0.6624070996689898</v>
+      </c>
+      <c r="F4">
+        <v>0.5931136172727171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.6518704867378313</v>
+      </c>
+      <c r="C5">
+        <v>0.6426551667835766</v>
+      </c>
+      <c r="D5">
+        <v>0.5238092652430802</v>
+      </c>
+      <c r="E5">
+        <v>0.5603799167002674</v>
+      </c>
+      <c r="F5">
+        <v>0.4940007909036573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5615059656494029</v>
+      </c>
+      <c r="C6">
+        <v>0.5868030349534594</v>
+      </c>
+      <c r="D6">
+        <v>0.5512174339563617</v>
+      </c>
+      <c r="E6">
+        <v>0.5672789858135707</v>
+      </c>
+      <c r="F6">
+        <v>0.5246822023761311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.6326568412635906</v>
+      </c>
+      <c r="C7">
+        <v>0.5799050553612939</v>
+      </c>
+      <c r="D7">
+        <v>0.6074179591259434</v>
+      </c>
+      <c r="E7">
+        <v>0.4955689465106738</v>
+      </c>
+      <c r="F7">
+        <v>0.5108329351422098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.650962489838551</v>
+      </c>
+      <c r="C8">
+        <v>0.6460789443042859</v>
+      </c>
+      <c r="D8">
+        <v>0.5499393338881162</v>
+      </c>
+      <c r="E8">
+        <v>0.6023989441400958</v>
+      </c>
+      <c r="F8">
+        <v>0.5963908442639059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabu search partially repaired,
</commit_message>
<xml_diff>
--- a/Wyniki/Tabele/jakosc_gleby.xlsx
+++ b/Wyniki/Tabele/jakosc_gleby.xlsx
@@ -419,13 +419,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.230729401521877</v>
+        <v>0.2316763795256406</v>
       </c>
       <c r="C2">
-        <v>0.2465603647703832</v>
+        <v>0.2830683067390554</v>
       </c>
       <c r="D2">
-        <v>0.2308905922386382</v>
+        <v>0.2144229011851627</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -433,13 +433,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2592440671686274</v>
+        <v>0.273196450901372</v>
       </c>
       <c r="C3">
-        <v>0.2373354381457112</v>
+        <v>0.2788866191901092</v>
       </c>
       <c r="D3">
-        <v>0.2206338793535892</v>
+        <v>0.2840676161439734</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -447,13 +447,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2629731166730794</v>
+        <v>0.2186905015119305</v>
       </c>
       <c r="C4">
-        <v>0.2251641719748579</v>
+        <v>0.2278386555315274</v>
       </c>
       <c r="D4">
-        <v>0.2386015002888902</v>
+        <v>0.2324696936659122</v>
       </c>
     </row>
   </sheetData>
@@ -488,13 +488,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5383686035510462</v>
+        <v>0.5405782188931615</v>
       </c>
       <c r="C2">
-        <v>0.5753075177975608</v>
+        <v>0.6604927157244626</v>
       </c>
       <c r="D2">
-        <v>0.5387447152234891</v>
+        <v>0.5003201027653797</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -502,13 +502,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.604902823393464</v>
+        <v>0.6374583854365347</v>
       </c>
       <c r="C3">
-        <v>0.5537826890066595</v>
+        <v>0.6507354447769214</v>
       </c>
       <c r="D3">
-        <v>0.5148123851583749</v>
+        <v>0.6628244376692711</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -516,13 +516,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.613603938903852</v>
+        <v>0.5102778368611712</v>
       </c>
       <c r="C4">
-        <v>0.525383067941335</v>
+        <v>0.5316235295735638</v>
       </c>
       <c r="D4">
-        <v>0.5567368340074105</v>
+        <v>0.5424292852204617</v>
       </c>
     </row>
   </sheetData>
@@ -557,13 +557,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7690980050729233</v>
+        <v>0.7722545984188022</v>
       </c>
       <c r="C2">
-        <v>0.8218678825679442</v>
+        <v>0.9435610224635179</v>
       </c>
       <c r="D2">
-        <v>0.7696353074621274</v>
+        <v>0.7147430039505425</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -571,13 +571,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.8641468905620915</v>
+        <v>0.9106548363379067</v>
       </c>
       <c r="C3">
-        <v>0.7911181271523708</v>
+        <v>0.9296220639670305</v>
       </c>
       <c r="D3">
-        <v>0.7354462645119642</v>
+        <v>0.9468920538132446</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -585,13 +585,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.8765770555769314</v>
+        <v>0.7289683383731018</v>
       </c>
       <c r="C4">
-        <v>0.750547239916193</v>
+        <v>0.7594621851050913</v>
       </c>
       <c r="D4">
-        <v>0.7953383342963007</v>
+        <v>0.7748989788863739</v>
       </c>
     </row>
   </sheetData>
@@ -626,13 +626,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.230729401521877</v>
+        <v>0.2316763795256406</v>
       </c>
       <c r="C2">
-        <v>0.2465603647703832</v>
+        <v>0.2830683067390554</v>
       </c>
       <c r="D2">
-        <v>0.2308905922386382</v>
+        <v>0.2144229011851627</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -640,13 +640,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2592440671686274</v>
+        <v>0.273196450901372</v>
       </c>
       <c r="C3">
-        <v>0.2373354381457112</v>
+        <v>0.2788866191901092</v>
       </c>
       <c r="D3">
-        <v>0.2206338793535892</v>
+        <v>0.2840676161439734</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -654,13 +654,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2629731166730794</v>
+        <v>0.2186905015119305</v>
       </c>
       <c r="C4">
-        <v>0.2251641719748579</v>
+        <v>0.2278386555315274</v>
       </c>
       <c r="D4">
-        <v>0.2386015002888902</v>
+        <v>0.2324696936659122</v>
       </c>
     </row>
   </sheetData>
@@ -695,13 +695,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.230729401521877</v>
+        <v>0.2316763795256406</v>
       </c>
       <c r="C2">
-        <v>0.2465603647703832</v>
+        <v>0.2830683067390554</v>
       </c>
       <c r="D2">
-        <v>0.2308905922386382</v>
+        <v>0.2144229011851627</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -709,13 +709,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2592440671686274</v>
+        <v>0.273196450901372</v>
       </c>
       <c r="C3">
-        <v>0.2373354381457112</v>
+        <v>0.2788866191901092</v>
       </c>
       <c r="D3">
-        <v>0.2206338793535892</v>
+        <v>0.2840676161439734</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -723,13 +723,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2629731166730794</v>
+        <v>0.2186905015119305</v>
       </c>
       <c r="C4">
-        <v>0.2251641719748579</v>
+        <v>0.2278386555315274</v>
       </c>
       <c r="D4">
-        <v>0.2386015002888902</v>
+        <v>0.2324696936659122</v>
       </c>
     </row>
   </sheetData>
@@ -764,13 +764,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7690980050729233</v>
+        <v>0.7722545984188022</v>
       </c>
       <c r="C2">
-        <v>0.8218678825679442</v>
+        <v>0.9435610224635179</v>
       </c>
       <c r="D2">
-        <v>0.7696353074621274</v>
+        <v>0.7147430039505425</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -778,13 +778,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.8641468905620915</v>
+        <v>0.9106548363379067</v>
       </c>
       <c r="C3">
-        <v>0.7911181271523708</v>
+        <v>0.9296220639670305</v>
       </c>
       <c r="D3">
-        <v>0.7354462645119642</v>
+        <v>0.9468920538132446</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -792,13 +792,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.8765770555769314</v>
+        <v>0.7289683383731018</v>
       </c>
       <c r="C4">
-        <v>0.750547239916193</v>
+        <v>0.7594621851050913</v>
       </c>
       <c r="D4">
-        <v>0.7953383342963007</v>
+        <v>0.7748989788863739</v>
       </c>
     </row>
   </sheetData>
@@ -833,13 +833,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5383686035510462</v>
+        <v>0.5405782188931615</v>
       </c>
       <c r="C2">
-        <v>0.5753075177975608</v>
+        <v>0.6604927157244626</v>
       </c>
       <c r="D2">
-        <v>0.5387447152234891</v>
+        <v>0.5003201027653797</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -847,13 +847,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.604902823393464</v>
+        <v>0.6374583854365347</v>
       </c>
       <c r="C3">
-        <v>0.5537826890066595</v>
+        <v>0.6507354447769214</v>
       </c>
       <c r="D3">
-        <v>0.5148123851583749</v>
+        <v>0.6628244376692711</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -861,13 +861,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.613603938903852</v>
+        <v>0.5102778368611712</v>
       </c>
       <c r="C4">
-        <v>0.525383067941335</v>
+        <v>0.5316235295735638</v>
       </c>
       <c r="D4">
-        <v>0.5567368340074105</v>
+        <v>0.5424292852204617</v>
       </c>
     </row>
   </sheetData>
@@ -902,13 +902,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5383686035510462</v>
+        <v>0.5405782188931615</v>
       </c>
       <c r="C2">
-        <v>0.5753075177975608</v>
+        <v>0.6604927157244626</v>
       </c>
       <c r="D2">
-        <v>0.5387447152234891</v>
+        <v>0.5003201027653797</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -916,13 +916,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.604902823393464</v>
+        <v>0.6374583854365347</v>
       </c>
       <c r="C3">
-        <v>0.5537826890066595</v>
+        <v>0.6507354447769214</v>
       </c>
       <c r="D3">
-        <v>0.5148123851583749</v>
+        <v>0.6628244376692711</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -930,13 +930,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.613603938903852</v>
+        <v>0.5102778368611712</v>
       </c>
       <c r="C4">
-        <v>0.525383067941335</v>
+        <v>0.5316235295735638</v>
       </c>
       <c r="D4">
-        <v>0.5567368340074105</v>
+        <v>0.5424292852204617</v>
       </c>
     </row>
   </sheetData>
@@ -971,13 +971,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5383686035510462</v>
+        <v>0.5405782188931615</v>
       </c>
       <c r="C2">
-        <v>0.5753075177975608</v>
+        <v>0.6604927157244626</v>
       </c>
       <c r="D2">
-        <v>0.5387447152234891</v>
+        <v>0.5003201027653797</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -985,13 +985,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.604902823393464</v>
+        <v>0.6374583854365347</v>
       </c>
       <c r="C3">
-        <v>0.5537826890066595</v>
+        <v>0.6507354447769214</v>
       </c>
       <c r="D3">
-        <v>0.5148123851583749</v>
+        <v>0.6628244376692711</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -999,13 +999,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.613603938903852</v>
+        <v>0.5102778368611712</v>
       </c>
       <c r="C4">
-        <v>0.525383067941335</v>
+        <v>0.5316235295735638</v>
       </c>
       <c r="D4">
-        <v>0.5567368340074105</v>
+        <v>0.5424292852204617</v>
       </c>
     </row>
   </sheetData>
@@ -1040,13 +1040,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7690980050729233</v>
+        <v>0.7722545984188022</v>
       </c>
       <c r="C2">
-        <v>0.8218678825679442</v>
+        <v>0.9435610224635179</v>
       </c>
       <c r="D2">
-        <v>0.7696353074621274</v>
+        <v>0.7147430039505425</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1054,13 +1054,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.8641468905620915</v>
+        <v>0.9106548363379067</v>
       </c>
       <c r="C3">
-        <v>0.7911181271523708</v>
+        <v>0.9296220639670305</v>
       </c>
       <c r="D3">
-        <v>0.7354462645119642</v>
+        <v>0.9468920538132446</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1068,13 +1068,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.8765770555769314</v>
+        <v>0.7289683383731018</v>
       </c>
       <c r="C4">
-        <v>0.750547239916193</v>
+        <v>0.7594621851050913</v>
       </c>
       <c r="D4">
-        <v>0.7953383342963007</v>
+        <v>0.7748989788863739</v>
       </c>
     </row>
   </sheetData>
@@ -1109,13 +1109,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5383686035510462</v>
+        <v>0.5405782188931615</v>
       </c>
       <c r="C2">
-        <v>0.5753075177975608</v>
+        <v>0.6604927157244626</v>
       </c>
       <c r="D2">
-        <v>0.5387447152234891</v>
+        <v>0.5003201027653797</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1123,13 +1123,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.604902823393464</v>
+        <v>0.6374583854365347</v>
       </c>
       <c r="C3">
-        <v>0.5537826890066595</v>
+        <v>0.6507354447769214</v>
       </c>
       <c r="D3">
-        <v>0.5148123851583749</v>
+        <v>0.6628244376692711</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1137,13 +1137,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.613603938903852</v>
+        <v>0.5102778368611712</v>
       </c>
       <c r="C4">
-        <v>0.525383067941335</v>
+        <v>0.5316235295735638</v>
       </c>
       <c r="D4">
-        <v>0.5567368340074105</v>
+        <v>0.5424292852204617</v>
       </c>
     </row>
   </sheetData>
@@ -1178,13 +1178,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5383686035510462</v>
+        <v>0.5405782188931615</v>
       </c>
       <c r="C2">
-        <v>0.5753075177975608</v>
+        <v>0.6604927157244626</v>
       </c>
       <c r="D2">
-        <v>0.5387447152234891</v>
+        <v>0.5003201027653797</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1192,13 +1192,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.604902823393464</v>
+        <v>0.6374583854365347</v>
       </c>
       <c r="C3">
-        <v>0.5537826890066595</v>
+        <v>0.6507354447769214</v>
       </c>
       <c r="D3">
-        <v>0.5148123851583749</v>
+        <v>0.6628244376692711</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1206,13 +1206,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.613603938903852</v>
+        <v>0.5102778368611712</v>
       </c>
       <c r="C4">
-        <v>0.525383067941335</v>
+        <v>0.5316235295735638</v>
       </c>
       <c r="D4">
-        <v>0.5567368340074105</v>
+        <v>0.5424292852204617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes, sol generator and much more
</commit_message>
<xml_diff>
--- a/Wyniki/Tabele/jakosc_gleby.xlsx
+++ b/Wyniki/Tabele/jakosc_gleby.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="4">
   <si>
     <t>Pole</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Nebbiolo</t>
-  </si>
-  <si>
-    <t>Arneis</t>
-  </si>
-  <si>
-    <t>Cortese</t>
   </si>
 </sst>
 </file>
@@ -400,13 +394,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,71 +413,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2234051819868965</v>
+        <v>0.2329558243663601</v>
       </c>
       <c r="C2">
-        <v>0.2149364649629517</v>
+        <v>0.2833027582515192</v>
       </c>
       <c r="D2">
-        <v>0.2339483208391916</v>
-      </c>
-      <c r="E2">
-        <v>0.2135075646742117</v>
-      </c>
-      <c r="F2">
-        <v>0.2649472464475501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.2652670960063206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2390995058042341</v>
+        <v>0.2310151984207836</v>
       </c>
       <c r="C3">
-        <v>0.2471625764861336</v>
+        <v>0.2783923921526206</v>
       </c>
       <c r="D3">
-        <v>0.215599032271489</v>
-      </c>
-      <c r="E3">
-        <v>0.2527949006049433</v>
-      </c>
-      <c r="F3">
-        <v>0.2298731242264698</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.2249564733308241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2159484075809939</v>
+        <v>0.23878809189623</v>
       </c>
       <c r="C4">
-        <v>0.2756051107880783</v>
+        <v>0.258915452273863</v>
       </c>
       <c r="D4">
-        <v>0.2744451299142301</v>
-      </c>
-      <c r="E4">
-        <v>0.2713482268796872</v>
-      </c>
-      <c r="F4">
-        <v>0.2565872809676555</v>
+        <v>0.2175118438881647</v>
       </c>
     </row>
   </sheetData>
@@ -493,13 +463,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,71 +482,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.446810363973793</v>
+        <v>0.5435635901881735</v>
       </c>
       <c r="C2">
-        <v>0.4298729299259035</v>
+        <v>0.6610397692535448</v>
       </c>
       <c r="D2">
-        <v>0.4678966416783833</v>
-      </c>
-      <c r="E2">
-        <v>0.4270151293484234</v>
-      </c>
-      <c r="F2">
-        <v>0.5298944928951003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.6189565573480814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.4781990116084682</v>
+        <v>0.5390354629818283</v>
       </c>
       <c r="C3">
-        <v>0.4943251529722672</v>
+        <v>0.6495822483561148</v>
       </c>
       <c r="D3">
-        <v>0.4311980645429781</v>
-      </c>
-      <c r="E3">
-        <v>0.5055898012098866</v>
-      </c>
-      <c r="F3">
-        <v>0.4597462484529395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.524898437771923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4318968151619879</v>
+        <v>0.5571722144245366</v>
       </c>
       <c r="C4">
-        <v>0.5512102215761566</v>
+        <v>0.6041360553056804</v>
       </c>
       <c r="D4">
-        <v>0.5488902598284602</v>
-      </c>
-      <c r="E4">
-        <v>0.5426964537593745</v>
-      </c>
-      <c r="F4">
-        <v>0.5131745619353111</v>
+        <v>0.507527635739051</v>
       </c>
     </row>
   </sheetData>
@@ -586,13 +532,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,71 +551,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7446839399563218</v>
+        <v>0.7765194145545335</v>
       </c>
       <c r="C2">
-        <v>0.7164548832098392</v>
+        <v>0.944342527505064</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0.7116918822473723</v>
-      </c>
-      <c r="F2">
-        <v>0.8831574881585005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.8842236533544021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.7969983526807805</v>
+        <v>0.7700506614026119</v>
       </c>
       <c r="C3">
-        <v>0.8238752549537787</v>
+        <v>0.9279746405087355</v>
       </c>
       <c r="D3">
-        <v>0.7186634409049635</v>
-      </c>
-      <c r="E3">
-        <v>0.8426496686831444</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.7498549111027472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7198280252699798</v>
+        <v>0.7959603063207666</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.8630515075795435</v>
       </c>
       <c r="D4">
-        <v>0.9148170997141003</v>
-      </c>
-      <c r="E4">
-        <v>0.9044940895989575</v>
-      </c>
-      <c r="F4">
-        <v>0.8552909365588519</v>
+        <v>0.7250394796272157</v>
       </c>
     </row>
   </sheetData>
@@ -679,13 +601,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,71 +620,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2234051819868965</v>
+        <v>0.2329558243663601</v>
       </c>
       <c r="C2">
-        <v>0.2149364649629517</v>
+        <v>0.2833027582515192</v>
       </c>
       <c r="D2">
-        <v>0.2339483208391916</v>
-      </c>
-      <c r="E2">
-        <v>0.2135075646742117</v>
-      </c>
-      <c r="F2">
-        <v>0.2649472464475501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.2652670960063206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2390995058042341</v>
+        <v>0.2310151984207836</v>
       </c>
       <c r="C3">
-        <v>0.2471625764861336</v>
+        <v>0.2783923921526206</v>
       </c>
       <c r="D3">
-        <v>0.215599032271489</v>
-      </c>
-      <c r="E3">
-        <v>0.2527949006049433</v>
-      </c>
-      <c r="F3">
-        <v>0.2298731242264698</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.2249564733308241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2159484075809939</v>
+        <v>0.23878809189623</v>
       </c>
       <c r="C4">
-        <v>0.2756051107880783</v>
+        <v>0.258915452273863</v>
       </c>
       <c r="D4">
-        <v>0.2744451299142301</v>
-      </c>
-      <c r="E4">
-        <v>0.2713482268796872</v>
-      </c>
-      <c r="F4">
-        <v>0.2565872809676555</v>
+        <v>0.2175118438881647</v>
       </c>
     </row>
   </sheetData>
@@ -772,13 +670,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,71 +689,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2234051819868965</v>
+        <v>0.2329558243663601</v>
       </c>
       <c r="C2">
-        <v>0.2149364649629517</v>
+        <v>0.2833027582515192</v>
       </c>
       <c r="D2">
-        <v>0.2339483208391916</v>
-      </c>
-      <c r="E2">
-        <v>0.2135075646742117</v>
-      </c>
-      <c r="F2">
-        <v>0.2649472464475501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.2652670960063206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.2390995058042341</v>
+        <v>0.2310151984207836</v>
       </c>
       <c r="C3">
-        <v>0.2471625764861336</v>
+        <v>0.2783923921526206</v>
       </c>
       <c r="D3">
-        <v>0.215599032271489</v>
-      </c>
-      <c r="E3">
-        <v>0.2527949006049433</v>
-      </c>
-      <c r="F3">
-        <v>0.2298731242264698</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.2249564733308241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.2159484075809939</v>
+        <v>0.23878809189623</v>
       </c>
       <c r="C4">
-        <v>0.2756051107880783</v>
+        <v>0.258915452273863</v>
       </c>
       <c r="D4">
-        <v>0.2744451299142301</v>
-      </c>
-      <c r="E4">
-        <v>0.2713482268796872</v>
-      </c>
-      <c r="F4">
-        <v>0.2565872809676555</v>
+        <v>0.2175118438881647</v>
       </c>
     </row>
   </sheetData>
@@ -865,13 +739,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,71 +758,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.7446839399563218</v>
+        <v>0.7765194145545335</v>
       </c>
       <c r="C2">
-        <v>0.7164548832098392</v>
+        <v>0.944342527505064</v>
       </c>
       <c r="D2">
-        <v>0.7798277361306388</v>
-      </c>
-      <c r="E2">
-        <v>0.7116918822473723</v>
-      </c>
-      <c r="F2">
-        <v>0.8831574881585005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.8842236533544021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.7969983526807805</v>
+        <v>0.7700506614026119</v>
       </c>
       <c r="C3">
-        <v>0.8238752549537787</v>
+        <v>0.9279746405087355</v>
       </c>
       <c r="D3">
-        <v>0.7186634409049635</v>
-      </c>
-      <c r="E3">
-        <v>0.8426496686831444</v>
-      </c>
-      <c r="F3">
-        <v>0.766243747421566</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.7498549111027472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7198280252699798</v>
+        <v>0.7959603063207666</v>
       </c>
       <c r="C4">
-        <v>0.9186837026269277</v>
+        <v>0.8630515075795435</v>
       </c>
       <c r="D4">
-        <v>0.9148170997141003</v>
-      </c>
-      <c r="E4">
-        <v>0.9044940895989575</v>
-      </c>
-      <c r="F4">
-        <v>0.8552909365588519</v>
+        <v>0.7250394796272157</v>
       </c>
     </row>
   </sheetData>
@@ -958,13 +808,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,71 +827,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.446810363973793</v>
+        <v>0.5435635901881735</v>
       </c>
       <c r="C2">
-        <v>0.4298729299259035</v>
+        <v>0.6610397692535448</v>
       </c>
       <c r="D2">
-        <v>0.4678966416783833</v>
-      </c>
-      <c r="E2">
-        <v>0.4270151293484234</v>
-      </c>
-      <c r="F2">
-        <v>0.5298944928951003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.6189565573480814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.4781990116084682</v>
+        <v>0.5390354629818283</v>
       </c>
       <c r="C3">
-        <v>0.4943251529722672</v>
+        <v>0.6495822483561148</v>
       </c>
       <c r="D3">
-        <v>0.4311980645429781</v>
-      </c>
-      <c r="E3">
-        <v>0.5055898012098866</v>
-      </c>
-      <c r="F3">
-        <v>0.4597462484529395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.524898437771923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4318968151619879</v>
+        <v>0.5571722144245366</v>
       </c>
       <c r="C4">
-        <v>0.5512102215761566</v>
+        <v>0.6041360553056804</v>
       </c>
       <c r="D4">
-        <v>0.5488902598284602</v>
-      </c>
-      <c r="E4">
-        <v>0.5426964537593745</v>
-      </c>
-      <c r="F4">
-        <v>0.5131745619353111</v>
+        <v>0.507527635739051</v>
       </c>
     </row>
   </sheetData>
@@ -1051,13 +877,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,71 +896,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.446810363973793</v>
+        <v>0.5435635901881735</v>
       </c>
       <c r="C2">
-        <v>0.4298729299259035</v>
+        <v>0.6610397692535448</v>
       </c>
       <c r="D2">
-        <v>0.4678966416783833</v>
-      </c>
-      <c r="E2">
-        <v>0.4270151293484234</v>
-      </c>
-      <c r="F2">
-        <v>0.5298944928951003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.6189565573480814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.4781990116084682</v>
+        <v>0.5390354629818283</v>
       </c>
       <c r="C3">
-        <v>0.4943251529722672</v>
+        <v>0.6495822483561148</v>
       </c>
       <c r="D3">
-        <v>0.4311980645429781</v>
-      </c>
-      <c r="E3">
-        <v>0.5055898012098866</v>
-      </c>
-      <c r="F3">
-        <v>0.4597462484529395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.524898437771923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4318968151619879</v>
+        <v>0.5571722144245366</v>
       </c>
       <c r="C4">
-        <v>0.5512102215761566</v>
+        <v>0.6041360553056804</v>
       </c>
       <c r="D4">
-        <v>0.5488902598284602</v>
-      </c>
-      <c r="E4">
-        <v>0.5426964537593745</v>
-      </c>
-      <c r="F4">
-        <v>0.5131745619353111</v>
+        <v>0.507527635739051</v>
       </c>
     </row>
   </sheetData>
@@ -1144,13 +946,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,71 +965,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.446810363973793</v>
+        <v>0.5435635901881735</v>
       </c>
       <c r="C2">
-        <v>0.4298729299259035</v>
+        <v>0.6610397692535448</v>
       </c>
       <c r="D2">
-        <v>0.4678966416783833</v>
-      </c>
-      <c r="E2">
-        <v>0.4270151293484234</v>
-      </c>
-      <c r="F2">
-        <v>0.5298944928951003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.6189565573480814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.4781990116084682</v>
+        <v>0.5390354629818283</v>
       </c>
       <c r="C3">
-        <v>0.4943251529722672</v>
+        <v>0.6495822483561148</v>
       </c>
       <c r="D3">
-        <v>0.4311980645429781</v>
-      </c>
-      <c r="E3">
-        <v>0.5055898012098866</v>
-      </c>
-      <c r="F3">
-        <v>0.4597462484529395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.524898437771923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4318968151619879</v>
+        <v>0.5571722144245366</v>
       </c>
       <c r="C4">
-        <v>0.5512102215761566</v>
+        <v>0.6041360553056804</v>
       </c>
       <c r="D4">
-        <v>0.5488902598284602</v>
-      </c>
-      <c r="E4">
-        <v>0.5426964537593745</v>
-      </c>
-      <c r="F4">
-        <v>0.5131745619353111</v>
+        <v>0.507527635739051</v>
       </c>
     </row>
   </sheetData>
@@ -1237,13 +1015,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1256,71 +1034,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.9946839399563218</v>
+        <v>0.7765194145545335</v>
       </c>
       <c r="C2">
-        <v>0.7164548832098392</v>
+        <v>0.944342527505064</v>
       </c>
       <c r="D2">
-        <v>0.7798277361306388</v>
-      </c>
-      <c r="E2">
-        <v>0.7116918822473723</v>
-      </c>
-      <c r="F2">
-        <v>0.8831574881585005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.8842236533544021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.7969983526807805</v>
+        <v>0.7700506614026119</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.9279746405087355</v>
       </c>
       <c r="D3">
-        <v>0.7186634409049635</v>
-      </c>
-      <c r="E3">
-        <v>0.8426496686831444</v>
-      </c>
-      <c r="F3">
-        <v>0.766243747421566</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.7498549111027472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.7198280252699798</v>
+        <v>0.7959603063207666</v>
       </c>
       <c r="C4">
-        <v>0.9186837026269277</v>
+        <v>0.8630515075795435</v>
       </c>
       <c r="D4">
-        <v>0.9148170997141003</v>
-      </c>
-      <c r="E4">
-        <v>0.9044940895989575</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>0.7250394796272157</v>
       </c>
     </row>
   </sheetData>
@@ -1330,13 +1084,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,71 +1103,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.446810363973793</v>
+        <v>0.5435635901881735</v>
       </c>
       <c r="C2">
-        <v>0.4298729299259035</v>
+        <v>0.6610397692535448</v>
       </c>
       <c r="D2">
-        <v>0.4678966416783833</v>
-      </c>
-      <c r="E2">
-        <v>0.4270151293484234</v>
-      </c>
-      <c r="F2">
-        <v>0.5298944928951003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.6189565573480814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.4781990116084682</v>
+        <v>0.5390354629818283</v>
       </c>
       <c r="C3">
-        <v>0.4943251529722672</v>
+        <v>0.6495822483561148</v>
       </c>
       <c r="D3">
-        <v>0.4311980645429781</v>
-      </c>
-      <c r="E3">
-        <v>0.5055898012098866</v>
-      </c>
-      <c r="F3">
-        <v>0.4597462484529395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.524898437771923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4318968151619879</v>
+        <v>0.5571722144245366</v>
       </c>
       <c r="C4">
-        <v>0.5512102215761566</v>
+        <v>0.6041360553056804</v>
       </c>
       <c r="D4">
-        <v>0.5488902598284602</v>
-      </c>
-      <c r="E4">
-        <v>0.5426964537593745</v>
-      </c>
-      <c r="F4">
-        <v>0.5131745619353111</v>
+        <v>0.507527635739051</v>
       </c>
     </row>
   </sheetData>
@@ -1423,13 +1153,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1442,71 +1172,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.446810363973793</v>
+        <v>0.5435635901881735</v>
       </c>
       <c r="C2">
-        <v>0.4298729299259035</v>
+        <v>0.6610397692535448</v>
       </c>
       <c r="D2">
-        <v>0.4678966416783833</v>
-      </c>
-      <c r="E2">
-        <v>0.4270151293484234</v>
-      </c>
-      <c r="F2">
-        <v>0.5298944928951003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.6189565573480814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.4781990116084682</v>
+        <v>0.5390354629818283</v>
       </c>
       <c r="C3">
-        <v>0.4943251529722672</v>
+        <v>0.6495822483561148</v>
       </c>
       <c r="D3">
-        <v>0.4311980645429781</v>
-      </c>
-      <c r="E3">
-        <v>0.5055898012098866</v>
-      </c>
-      <c r="F3">
-        <v>0.4597462484529395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.524898437771923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4318968151619879</v>
+        <v>0.5571722144245366</v>
       </c>
       <c r="C4">
-        <v>0.5512102215761566</v>
+        <v>0.6041360553056804</v>
       </c>
       <c r="D4">
-        <v>0.5488902598284602</v>
-      </c>
-      <c r="E4">
-        <v>0.5426964537593745</v>
-      </c>
-      <c r="F4">
-        <v>0.5131745619353111</v>
+        <v>0.507527635739051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>